<commit_message>
adding excel_reader.py and updated the data in xlsx files.
</commit_message>
<xml_diff>
--- a/rai/rai.xlsx
+++ b/rai/rai.xlsx
@@ -10,12 +10,25 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="8_{221786BB-C0D1-4A24-ACDA-35161C0B9440}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="480" windowWidth="21840" windowHeight="38040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="480" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="World" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" iterate="1" calcOnSave="0" concurrentManualCount="24"/>
+  <calcPr calcId="191029" iterate="1" calcOnSave="0" concurrentManualCount="24"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -7702,8 +7715,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C2432"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+    <sheetView tabSelected="1" topLeftCell="A2378" workbookViewId="0">
+      <selection activeCell="A2432" sqref="A2432"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
updating the data to 5/13/2025
</commit_message>
<xml_diff>
--- a/rai/rai.xlsx
+++ b/rai/rai.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c060ac0a7f9c7ae2/main/DELL_NB/TAA/rai/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c060ac0a7f9c7ae2/main/CRAMC_Desktop/TAA/rai/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{221786BB-C0D1-4A24-ACDA-35161C0B9440}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{221786BB-C0D1-4A24-ACDA-35161C0B9440}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{36CA3634-70A5-498C-9990-899633FF50A3}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="480" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="480" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="World" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2434" uniqueCount="2434">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2444" uniqueCount="2444">
   <si>
     <t>Date</t>
   </si>
@@ -7335,6 +7335,36 @@
   </si>
   <si>
     <t>2025-04-25</t>
+  </si>
+  <si>
+    <t>2025-04-28</t>
+  </si>
+  <si>
+    <t>2025-04-29</t>
+  </si>
+  <si>
+    <t>2025-04-30</t>
+  </si>
+  <si>
+    <t>2025-05-01</t>
+  </si>
+  <si>
+    <t>2025-05-02</t>
+  </si>
+  <si>
+    <t>2025-05-05</t>
+  </si>
+  <si>
+    <t>2025-05-06</t>
+  </si>
+  <si>
+    <t>2025-05-07</t>
+  </si>
+  <si>
+    <t>2025-05-08</t>
+  </si>
+  <si>
+    <t>2025-05-09</t>
   </si>
 </sst>
 </file>
@@ -7376,9 +7406,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -7713,10 +7744,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2432"/>
+  <dimension ref="A1:C2442"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2378" workbookViewId="0">
-      <selection activeCell="A2432" sqref="A2432"/>
+    <sheetView tabSelected="1" topLeftCell="A2414" workbookViewId="0">
+      <selection activeCell="M2425" sqref="M2425"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -34476,6 +34507,116 @@
         <v>-0.25290000000000001</v>
       </c>
     </row>
+    <row r="2433" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2433" s="2" t="s">
+        <v>2434</v>
+      </c>
+      <c r="B2433" s="2">
+        <v>-0.74409999999999998</v>
+      </c>
+      <c r="C2433" s="2">
+        <v>-0.2717</v>
+      </c>
+    </row>
+    <row r="2434" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2434" s="2" t="s">
+        <v>2435</v>
+      </c>
+      <c r="B2434" s="2">
+        <v>-0.81420000000000003</v>
+      </c>
+      <c r="C2434" s="2">
+        <v>-0.30990000000000001</v>
+      </c>
+    </row>
+    <row r="2435" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2435" s="2" t="s">
+        <v>2436</v>
+      </c>
+      <c r="B2435" s="2">
+        <v>-0.88039999999999996</v>
+      </c>
+      <c r="C2435" s="2">
+        <v>-0.43319999999999997</v>
+      </c>
+    </row>
+    <row r="2436" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2436" s="2" t="s">
+        <v>2437</v>
+      </c>
+      <c r="B2436" s="2">
+        <v>-0.71989999999999998</v>
+      </c>
+      <c r="C2436" s="2">
+        <v>-0.33279999999999998</v>
+      </c>
+    </row>
+    <row r="2437" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2437" s="2" t="s">
+        <v>2438</v>
+      </c>
+      <c r="B2437" s="2">
+        <v>-0.47120000000000001</v>
+      </c>
+      <c r="C2437" s="2">
+        <v>-0.15190000000000001</v>
+      </c>
+    </row>
+    <row r="2438" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2438" s="2" t="s">
+        <v>2439</v>
+      </c>
+      <c r="B2438" s="2">
+        <v>-0.47370000000000001</v>
+      </c>
+      <c r="C2438" s="2">
+        <v>-0.1229</v>
+      </c>
+    </row>
+    <row r="2439" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2439" s="2" t="s">
+        <v>2440</v>
+      </c>
+      <c r="B2439" s="2">
+        <v>-0.45169999999999999</v>
+      </c>
+      <c r="C2439" s="2">
+        <v>-0.1426</v>
+      </c>
+    </row>
+    <row r="2440" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2440" s="2" t="s">
+        <v>2441</v>
+      </c>
+      <c r="B2440" s="2">
+        <v>-0.51</v>
+      </c>
+      <c r="C2440" s="2">
+        <v>-0.17430000000000001</v>
+      </c>
+    </row>
+    <row r="2441" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2441" s="2" t="s">
+        <v>2442</v>
+      </c>
+      <c r="B2441" s="2">
+        <v>-0.32269999999999999</v>
+      </c>
+      <c r="C2441" s="2">
+        <v>3.1899999999999998E-2</v>
+      </c>
+    </row>
+    <row r="2442" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2442" s="2" t="s">
+        <v>2443</v>
+      </c>
+      <c r="B2442" s="2">
+        <v>-0.2702</v>
+      </c>
+      <c r="C2442" s="2">
+        <v>8.5800000000000001E-2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>